<commit_message>
Creamos detalle del producto
</commit_message>
<xml_diff>
--- a/assets/php/listado.xlsx
+++ b/assets/php/listado.xlsx
@@ -1483,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
@@ -1617,7 +1617,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="15.35" customHeight="1">
@@ -1668,7 +1668,7 @@
         <v>24</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" ht="15.35" customHeight="1">
@@ -1719,7 +1719,7 @@
         <v>29</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" ht="15.35" customHeight="1">
@@ -1753,7 +1753,7 @@
         <v>32</v>
       </c>
       <c r="E17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" ht="15.35" customHeight="1">
@@ -1804,7 +1804,7 @@
         <v>36</v>
       </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" ht="15.35" customHeight="1">
@@ -1821,7 +1821,7 @@
         <v>39</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" ht="15.35" customHeight="1">
@@ -1957,7 +1957,7 @@
         <v>51</v>
       </c>
       <c r="E29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" ht="15.35" customHeight="1">
@@ -1974,7 +1974,7 @@
         <v>54</v>
       </c>
       <c r="E30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" ht="15.35" customHeight="1">
@@ -2025,7 +2025,7 @@
         <v>60</v>
       </c>
       <c r="E33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" ht="15.35" customHeight="1">
@@ -2042,7 +2042,7 @@
         <v>63</v>
       </c>
       <c r="E34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" ht="15.35" customHeight="1">
@@ -2161,7 +2161,7 @@
         <v>79</v>
       </c>
       <c r="E41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="15.35" customHeight="1">
@@ -2178,7 +2178,7 @@
         <v>81</v>
       </c>
       <c r="E42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" ht="15.35" customHeight="1">
@@ -2246,7 +2246,7 @@
         <v>89</v>
       </c>
       <c r="E46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" ht="15.35" customHeight="1">

</xml_diff>

<commit_message>
Actualizamos detalle de los productos
</commit_message>
<xml_diff>
--- a/assets/php/listado.xlsx
+++ b/assets/php/listado.xlsx
@@ -11,179 +11,170 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
-  <si>
-    <t>Ejes de Torsión</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+  <si>
+    <t>Eje de Torsión 4 Pernos 750 Kg.</t>
   </si>
   <si>
     <t>torsion</t>
   </si>
   <si>
-    <t>a. Eje de torsión|b. Abrazadera (Unión T)|c. Tubo para alargar eje de torsión</t>
-  </si>
-  <si>
-    <t>Eje de Torsión 4 Pernos 750 Kg.</t>
-  </si>
-  <si>
-    <t>Marca: AL-KO|Capacidad: 750 Kg. (1650 Lb.)|Fácil Instalación|&lt;br /&gt;|&lt;strong&gt;NO NECESITA&lt;/strong&gt;|• Paquetes de resorte|• Platineras|• Abrazaderas|• Orejas|• Uniones|• Monturitas|&lt;br /&gt;|&lt;strong&gt;BENEFICIOS:&lt;/strong&gt;|✓Amortiguación suave|✓Mayor estabilidad a mayor velocidad|✓No salta la carga|✓Se elimina el tiempo de armado y suelda del eje en el sistema convencional</t>
+    <t>Marca: AL-KO|Capacidad: 750 Kg. (1650 Lb.)|Fácil Instalación|Se adhiere al chasis mediante 8 pernos.|Garantía: 2 años.|&lt;br /&gt;|Al usar este eje de torsión, &lt;strong&gt;NO NECESITA&lt;/strong&gt;|• Paquetes de resorte|• Platineras|• Abrazaderas|• Orejas|• Uniones|• Monturitas|&lt;br /&gt;|&lt;strong&gt;BENEFICIOS:&lt;/strong&gt;|✓Amortiguación suave|✓Mayor estabilidad a mayor velocidad|✓No salta la carga|✓Se elimina el tiempo de armado y suelda del eje en el sistema convencional</t>
   </si>
   <si>
     <t>Eje de Torsión 5 Pernos 1000 Kg.</t>
   </si>
   <si>
-    <t>Capacidad: 1000 Kg. (2200 lb)|Fácil Instalación|NO NECESITA|Paquetes de resorte|Platineras|Abrazaderas|Orejas|Uniones|Monturitas|BENEFICIOS:|Amortiguación suave|Mayor estabilidad a mayor velocidad|No salta la carga|Se elimina el tiempo de armado y suelda del eje en el sistema convencional</t>
+    <t>Marca: AL-KO|Capacidad: 1000 Kg. (2200 lb)|Fácil Instalación|Se adhiere al chasis mediante 10 pernos.|Garantía: 2 años.|&lt;br /&gt;|Al usar este eje de torsión, &lt;strong&gt;NO NECESITA&lt;/strong&gt;|• Paquetes de resorte|• Platineras|• Abrazaderas|• Orejas|• Uniones|• Monturitas|&lt;br /&gt;|&lt;strong&gt;BENEFICIOS:&lt;/strong&gt;|✓Amortiguación suave|✓Mayor estabilidad a mayor velocidad|✓No salta la carga|✓Se elimina el tiempo de armado y suelda del eje en el sistema convencional</t>
   </si>
   <si>
     <t>Eje de Torsión 5 Pernos 1300 Kg.</t>
   </si>
   <si>
-    <t>Capacidad: 1300 Kg. (2860 lb)|Fácil Instalación|NO NECESITA|Paquetes de resorte|Platineras|Abrazaderas|Orejas|Uniones|Monturitas|BENEFICIOS:|Amortiguación suave|Mayor estabilidad a mayor velocidad|No salta la carga|Se elimina el tiempo de armado y suelda del eje en el sistema convencional</t>
+    <t>Marca: AL-KO|Capacidad: 1300 Kg. (2860 lb)|Fácil Instalación|Se adhiere al chasis mediante 10 pernos.|Garantía: 2 años.|&lt;br /&gt;|Al usar este eje de torsión, &lt;strong&gt;NO NECESITA&lt;/strong&gt;|• Paquetes de resorte|• Platineras|• Abrazaderas|• Orejas|• Uniones|• Monturitas|&lt;br /&gt;|&lt;strong&gt;BENEFICIOS:&lt;/strong&gt;|✓ Amortiguación suave|✓ Mayor estabilidad a mayor velocidad|✓ No salta la carga|✓ Se elimina el tiempo de armado y suelda del eje en el sistema convencional</t>
   </si>
   <si>
     <t>Abrazadera Union T</t>
   </si>
   <si>
-    <t>Sistema de Sujeción para armar Chasis T de 750 Kg.</t>
+    <t>Abrazaderas para instalación de Ejes de torsión en chasis de remolques.|Galvanizadas en caliente.|Incluye tornillería.|Marca: AL-KO</t>
   </si>
   <si>
     <t>Tubo de Eje de Torsión</t>
   </si>
   <si>
-    <t>Tubo original galvanizado|Capacidad 750 kg</t>
-  </si>
-  <si>
-    <t>Kit de Punta de Eje</t>
+    <t xml:space="preserve">Tramo de tubo exterior hexagonal para alargar ejes de torsión de 750 Kg.|Galvanizado en caliente.|Marca: AL-KO </t>
+  </si>
+  <si>
+    <t>Kit de Punta de Eje 4 Pernos 1000 Lb.</t>
   </si>
   <si>
     <t>punta</t>
   </si>
   <si>
-    <t>Kit de Punta de Eje 4 Pernos 1000 Lb.</t>
-  </si>
-  <si>
-    <t>Distancia entre pernos:|4" (10 cm. Aprox.)|"Incluye"|Rulimanes|Retenedor|Seguro|Tapa grasera|Tuercas de seguridad aceradas|Punta con tuerca y arandela.|Se necesitan 2 Kits para armar un eje de 2000 Lb.|Trabaja con aros de 12" - 13" - 14".</t>
+    <t>Distancia entre pernos: 4" (10 cm. Aprox.)|Se necesitan 2 Kits para armar un eje de 2000 Lb.|Trabaja con aros de 12”, 13”, 14".</t>
   </si>
   <si>
     <t>Kit de Punta de Eje 4 Pernos 1250 Lb.</t>
   </si>
   <si>
-    <t>Distancia entre pernos:|4" (10 cm. Aprox.)|"Incluye"|Rulimanes|Retenedor|Seguro|Tapa grasera|Tuercas de seguridad aceradas|Punta con tuerca y arandela.|Se necesitan 2 Kits para armar un eje de 2500 Lb.|Trabaja con aros de 12" - 13" - 14".</t>
+    <t xml:space="preserve">Distancia entre pernos: 4" (10 cm. Aprox.)|Se necesitan 2 Kits para armar un eje de 2500 Lb.|Trabaja con aros de 12”, 13”, 14". </t>
   </si>
   <si>
     <t>Kit de Punta de Eje 5 Pernos 1750 Lb.</t>
   </si>
   <si>
-    <t>Distancia entre pernos:|4.5" (11.40 cm. Aprox.)|"Incluye"|Rulimanes|Retenedor|Seguro|Tapa grasera|Tuercas de seguridad aceradas|Punta con tuerca y arandela.|Se necesitan 2 Kits para armar un eje de 3500 Lb.|Trabaja con aros de 14" - 15" - 16".</t>
+    <t xml:space="preserve">Distancia entre pernos: 4.5" (11.40 cm. Aprox.)|Se necesitan 2 Kits para armar un eje de 3500 Lb.|Trabaja con aros de 14”, 15”, 16". </t>
   </si>
   <si>
     <t>Kit de Punta de Eje 6 Pernos 3000 Lb.</t>
   </si>
   <si>
-    <t>Distancia entre pernos:|5.5" (14 cm. Aprox.)|"Incluye"|Rulimanes|Retenedor|Seguro|Tapa grasera|Tuercas de seguridad aceradas|Punta con tuerca y arandela.|Se necesitan 2 Kits para armar un eje de 6000 Lb.|Trabaja con aros de 14" - 15" - 16".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suspensión </t>
+    <t xml:space="preserve">Distancia entre pernos: 5.5" (14 cm. Aprox.)|Se necesitan 2 Kits para armar un eje de 6000 Lb.|Trabaja con aros de 14”, 15”, 16". </t>
+  </si>
+  <si>
+    <t>Paquetes de Resorte 1650 Lb.</t>
   </si>
   <si>
     <t>suspension</t>
   </si>
   <si>
-    <t>a. Paquetes de resorte|b. Kit de Orejas|c. Kit de Balanchines</t>
-  </si>
-  <si>
-    <t>Paquetes de Resorte</t>
-  </si>
-  <si>
-    <t>Paquete de Resorte 3 Hojas, de Un Solo Ojo|Capacidad: 1650 Lb.|Largo: 24 pulgadas.|Ancho: 1.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paquetes de Resorte </t>
-  </si>
-  <si>
-    <t>Paquete de Resorte 3 Hojas, de Un Doble Ojo|Capacidad: 1850 Lb.|Largo: 20 pulgadas.|Ancho: 1.75</t>
-  </si>
-  <si>
-    <t>Paquete de Resorte 5 Hojas, de Un Solo Ojo|Capacidad: 2300 Lb.|Largo: 29.5 pulgadas.|Ancho: 1.75</t>
-  </si>
-  <si>
-    <t>Paquete de Resorte 6 Hojas, de Un Doble Ojo|Capacidad: 3500 Lb.|Largo: 25 pulgadas.|Ancho: 1.75</t>
-  </si>
-  <si>
-    <t>Kit de Orejas</t>
-  </si>
-  <si>
-    <t>Conjunto de Pernos, Tuercas y Platineras|Para soldar al chasis e instalar los paquetes.</t>
-  </si>
-  <si>
-    <t>Para paquetes de UN SOLO OJO|Incluye:|2 Orejas 1 3/4 x 1 1/2|2 Uniones 3/4 x 2|2 Pernos 1/2 x 3 1/2 Galvanizados|Se Necesita 1 solo Kit para instalar 2 paquetes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para paquetes de DOBLE OJO|Incluye:|2 Orejas 3/4 x 1 1/2|2 Orejas 1 1/4 x 1 1/4|2 Platinas 1/2 x 3 1/2|6 Pernos con Tuercas 1/2 x 3 1/2|Se necesita 1 solo Kit para instalar 2 paquetes </t>
+    <t>Capacidad: 1650 Lb.|Largo: 24” (60.96 cm.)|Ancho: 1 3⁄4” (4.45 cm.)|(La distancia se mide del centro del ojo hasta el centro del final de la hoja.)</t>
+  </si>
+  <si>
+    <t>Paquetes de Resorte 1850 Lb.</t>
+  </si>
+  <si>
+    <t>Capacidad: 1850 Lb.|Largo: 20” (50.80 cm.)|Ancho: 1 3⁄4” (4.45 cm.)|(La distancia se mide de centro a centro de cada ojo.)</t>
+  </si>
+  <si>
+    <t>Paquetes de Resorte 2300 Lb.</t>
+  </si>
+  <si>
+    <t>Capacidad: 2300 Lb.|Largo: 29.5” (74.93 cm.)|Ancho: 1 3⁄4” (4.45 cm.)|(La distancia se mide del centro del ojo hasta el centro del final de la hoja.)</t>
+  </si>
+  <si>
+    <t>Paquetes de Resorte 3000 Lb.</t>
+  </si>
+  <si>
+    <t>Capacidad: 3500 Lb.|Largo: 25” (63.50 cm.)|Ancho: 1 3⁄4” (4.45 cm.)|(La distancia se mide de centro a centro de cada ojo.)</t>
+  </si>
+  <si>
+    <t>Kit de Orejas para un Solo Ojo</t>
+  </si>
+  <si>
+    <t>Sirven para paquetes de un solo ojo (deslizantes).|&lt;br /&gt;|&lt;strong&gt;Comprende:&lt;/strong&gt;|• 2 Orejas delanteras 1 3⁄4” X 1 1⁄2”|• 2 Uniones 3⁄4” x 2”|• 2 Pernos 1⁄2” X 3 1⁄2”|• 2 Tuercas 1⁄2|&lt;br /&gt;|Se necesita 1 solo kit para instalar 2 paquetes.</t>
+  </si>
+  <si>
+    <t>Kit de Orejas para Doble Ojo</t>
+  </si>
+  <si>
+    <t>Sirven para paquetes de doble ojo.|&lt;br /&gt;|&lt;strong&gt;Comprende:&lt;/strong&gt;|• 2 Orejas delanteras 1 3⁄4” X 1 1⁄2”|• 2 Orejas posteriores 1 1⁄4” x 1 1⁄4”|• 4 Platineras 1 1⁄2” x 1⁄4”|• 6 Pernos 1⁄2” X 3 1⁄2”|• 6 Tuercas 1⁄2|&lt;br /&gt;|Se necesita 1 solo kit para instalar 2 paquetes.</t>
   </si>
   <si>
     <t>Kit de Balancines</t>
   </si>
   <si>
-    <t>Kit de Balancines para armar sistema de doble eje.|Incluye:|4 Orejas 1 3/4 x 1 1/2|8 Platinas 1 1/2 x 1 1/4|2 Orejas de Balance|2 Triangulos de balance|14 Pernos 1/2 x 3 1/2|14 Tuercas 1/2|No incluye paquetes de Resorte.</t>
-  </si>
-  <si>
-    <t>Patas de Soporte</t>
+    <t>Sistema para instalar paquetes de resorte en remolques de doble eje.|&lt;br /&gt;|&lt;strong&gt;Comprende:&lt;/strong&gt;|• 4 Orejas delanteras 1 3⁄4” X 1 1⁄2”|• 2 Orejas de balance 2 1⁄4”|• 2 Triángulos de balance 7 3⁄4”|• 8 Platineras 1 1⁄2” x 1⁄4”|• 14 Pernos 1/2” x 3 1/2”|• 14 Tuercas 1/2|Se necesita 1 solo kit para instalar 4 paquetes.|No incluye paquetes de Resorte.</t>
+  </si>
+  <si>
+    <t>Patas de Soporte con Rueda - 1000 Lb.</t>
   </si>
   <si>
     <t>patas</t>
   </si>
   <si>
-    <t>a. Patas de soporte con rueda|b. Patas de soporte estáticas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patas de Soporte con Rueda </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pata Soporte con Rueda Plástica|Capacidad: 1000 Lb.|Medidas:|23" (58.42 cm.) en estado normal|34" (86.36 cm.) extendida|Utilidades:|Facilita el engache en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 40 cm.|Sirve como apoyo cuando el remolque está estacionado.|Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda. </t>
-  </si>
-  <si>
-    <t>Rueda Compacta|Capacidad: 150 Kg. Para remolques de 750 Kg.|Medidas:|50 cm. en estado normal|80 cm. extendida|Utilidades:|Facilita el engache en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 30 cm.|Sirve como apoyo cuando el remolque está estacionado.|Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda.</t>
-  </si>
-  <si>
-    <t>Patas Soporte con Llanta</t>
-  </si>
-  <si>
-    <t>Rueda Compacta|Capacidad: 200 Kg. Para remolques de 1000 Kg.|Medidas:|50 cm. en estado normal|85 cm. extendida|Utilidades:|Facilita el engache en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 35 cm.|Sirve como apoyo cuando el remolque está estacionado.|Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda.</t>
-  </si>
-  <si>
-    <t>Capacidad 300 Kg. Para remolques de 1500 Kg.|Medidas:|(57 cm.) Estado Normal|(87 cm.) Extendida|Utilidades:|Sube y baja 30 cm. Aprox.|Sirve como apoyo cuando el remolque está estacionado</t>
-  </si>
-  <si>
-    <t>Patas Soporte con Rueda</t>
-  </si>
-  <si>
-    <t>Capacidad 500 Kg. Para remolques de 2500 Kg.|Medidas:|(48 cm.) Estado Normal|(78 cm.) Extendida|Utilidades:|Sube y baja 30 cm. Aprox.|Sirve como apoyo cuando el remolque está estacionado</t>
-  </si>
-  <si>
-    <t>Patas Soporte Estacionarias</t>
-  </si>
-  <si>
-    <t>Capacidad 5000 Lb.|Medidas:|24.5" (63.50 cm.) Estado Normal|40" (104.14 cm.) Extendida|Utilidades:|Sube y baja 40 cm. aprox.|Sirve como apoyo cuando el remolque está estacionado</t>
-  </si>
-  <si>
-    <t>Capacidad 1000 Kg.|Para remolques de 2500 Kg.|Medidas:|54 cm. Estado Normal|90 cm. Extendida|Utilidades|Sube y baja 35 cm. aprox.|Sirve como apoyo cuando el remolque está estacionado</t>
-  </si>
-  <si>
-    <t>Capacidad 2500 Lb.|Medidas:|23" (58.42 cm.) Estado Normal|34" (86.36 cm.) Extendida|Utilidades:|Sube y baja 40 cm. Aprox.|Sirve como apoyo cuando el remolque está estacionado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aros con Llantas </t>
+    <t>Con rueda plástica.|&lt;strong&gt;Medidas:&lt;strong&gt;|23” (58.42 cm.) en estado normal|34” (86.36 cm.) extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|• Facilita el enganche en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 40 cm.|• Sirve como apoyo cuando el remolque está estacionado.|• Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda.</t>
+  </si>
+  <si>
+    <t>Patas de Soporte con Rueda - 750 Kg</t>
+  </si>
+  <si>
+    <t>Marca AL-KO.|Con rueda compacta.|&lt;strong&gt;Capacidad:&lt;/strong&gt; 150 Kg. Para remolques 750 Kg.|&lt;strong&gt;Medidas:&lt;strong&gt;|50 cm. en estado normal|80 cm. extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|•Facilita el enganche en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 30 cm.|•Sirve como apoyo cuando el remolque está estacionado.|•Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda.</t>
+  </si>
+  <si>
+    <t>Patas Soporte con Llanta - 1000 Kg.</t>
+  </si>
+  <si>
+    <t>Marca AL-KO.|&lt;strong&gt;Capacidad:&lt;/strong&gt; 200 Kg. Para remolques 1000 Kg.|&lt;strong&gt;Medidas:&lt;strong&gt;|50 cm. en estado normal|85 cm. extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|• Facilita el enganche en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 35 cm.|• Sirve como apoyo cuando el remolque está estacionado.|• Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda.</t>
+  </si>
+  <si>
+    <t>Patas Soporte con Rueda - 1500 Kg.</t>
+  </si>
+  <si>
+    <t>Marca AL-KO.|Con rueda compacta.|&lt;strong&gt;Capacidad:&lt;/strong&gt; 300 Kg. Para remolques 1500 Kg.|&lt;strong&gt;Medidas:&lt;strong&gt;|57 cm. en estado normal|87 cm. extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|•Facilita el enganche en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 30 cm.|•Sirve como apoyo cuando el remolque está estacionado.|•Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda.</t>
+  </si>
+  <si>
+    <t>Patas Soporte con Rueda - 2500 Kg.</t>
+  </si>
+  <si>
+    <t>Marca AL-KO.|Con rueda compacta.|&lt;strong&gt;Capacidad:&lt;/strong&gt; 500 Kg. Para remolques 2500 Kg.|&lt;strong&gt;Medidas:&lt;strong&gt;|48 cm. en estado normal|78 cm. extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|• Facilita el enganche en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 30 cm.|• Sirve como apoyo cuando el remolque está estacionado.|• Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda.</t>
+  </si>
+  <si>
+    <t>Patas Soporte Estacionarias - 1000 Kg.</t>
+  </si>
+  <si>
+    <t>Marca AL-KO.|Con base redonda.|&lt;strong&gt;Capacidad:&lt;/strong&gt; 1000 Kg. Para remolques 2000 Kg.|&lt;strong&gt;Medidas:&lt;strong&gt;|54 cm. en estado normal|90 cm. extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|• Facilita el enganche en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 36 cm.|• Sirve como apoyo cuando el remolque está estacionado.</t>
+  </si>
+  <si>
+    <t>Patas Soporte Estacionarias - 2500 Lb.</t>
+  </si>
+  <si>
+    <t>Con base cuadrada. Galvanizada.|Viene con pernos y platinas para instalar en el remolque.|&lt;strong&gt;Medidas:&lt;strong&gt;|24” (63.50 cm.) en estado normal|41” (104.14 cm.) extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|• Sube y baja 30 cm. Aprox.|•	Sirve como apoyo cuando el remolque está estacionado.</t>
+  </si>
+  <si>
+    <t>Patas Soporte Estacionarias - 5000 Lb.</t>
+  </si>
+  <si>
+    <t>Con base cuadrada. Galvanizada.|Viene con pernos y platinas para instalar en el remolque.|&lt;strong&gt;Medidas:&lt;strong&gt;|24.5” (62.23 cm.) en estado normal|40” (101.60 cm.) extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|• Sube y baja 40 cm. Aprox.|• Sirve como apoyo cuando el remolque está estacionado.</t>
+  </si>
+  <si>
+    <t>Aros con Llanta 8</t>
   </si>
   <si>
     <t>aros</t>
   </si>
   <si>
-    <t>a. Aros con llanta 8|b. Aros con llanta 12|c. Aros con llanta 14</t>
-  </si>
-  <si>
-    <t>Aros con Llanta 8</t>
-  </si>
-  <si>
     <t>4 Huecos|Medida llanta: 4.80 x 8.|Capacidad 585 Lb.|Aro Blanco</t>
   </si>
   <si>
@@ -199,85 +190,73 @@
     <t>5 Huecos|Medida llanta: ST205/75D14|Capacidad 1760 Lb.|Aro Blanco</t>
   </si>
   <si>
-    <t xml:space="preserve">Guardafangos </t>
+    <t>Guardafangos Sencillos</t>
   </si>
   <si>
     <t>guardafangos</t>
   </si>
   <si>
-    <t>a. Guardafangos sencillos ALKO|b. Guardafangos para doble eje ALKO</t>
-  </si>
-  <si>
-    <t>Guardafangos Sencillos</t>
-  </si>
-  <si>
-    <t>Plásticos Alemanes|ARO 13 - 14|Largo 73 cm.|Ancho 20 cm.|Profundidad: 36 cm.</t>
+    <t>Para un solo eje.|Marca: AL-KO.|Material: plástico|Trabajan con aro 13” y 14”. Largo 73 cm.|Ancho 20 cm.|Profundidad 36 cm.</t>
   </si>
   <si>
     <t>Guardafangos Dobles</t>
   </si>
   <si>
-    <t>Plásticos Alemanes|ARO 13 - 14 - 15|Largo 150 cm.|Ancho 22 cm.|Profundidad: 36 cm.</t>
-  </si>
-  <si>
-    <t>Sistema de Freno 7000 Lb.</t>
+    <t>Para doble eje.|Marca: AL-KO.|Material: plástico|Trabajan con aro 13” y 14”. Largo 146 cm.|Ancho 22 cm. Profundidad 36 cm.</t>
+  </si>
+  <si>
+    <t>Acople de freno</t>
   </si>
   <si>
     <t>frenos</t>
   </si>
   <si>
-    <t>El sistema de freno completo comprende:|Acople de freno|Frenos de disco|Puntas de eje|Mangueras.|Capacidad: 7000 lb. (3.1 toneladas)</t>
+    <t>Capacidad 7000 Lb. (3.1 Ton.)|Trabaja con bola 2”.|Solenoide incorporado al cilindro maestro, que facilita la revisión sin sacar la línea de frenado.|Con pin de seguridad para la bola, y cable de freno recubierto en PVC.</t>
   </si>
   <si>
     <t>Punta de Eje con Brida de Freno</t>
   </si>
   <si>
-    <t>1 3/8 x 1 1/16|Capacidad 3500 Lb.|Viene con tuerca y arandela|Cantidad requerida por eje: 2</t>
+    <t>1 3/8” x 1 1/16”|Capacidad 3500 Lb.|Con tuerca y arandela.|Cantidad requerida por eje: 2.</t>
   </si>
   <si>
     <t>Kit de Freno de Discos 10" para Remolque</t>
   </si>
   <si>
-    <t>Capacidad 7000 Lb. (3.1 toneladas)|Este Kit incluye:|2 Mordazas|2 Discos de freno 10 pulgadas|2 Soportes de morzada|Juego de rulimanes|Esas cantidades sirven para armar UN EJE.</t>
+    <t>Capacidad 7000 Lb. (3.1 Ton.)|&lt;br /&gt;|&lt;strong&gt;Este kit comprende:&lt;/strong&gt;|•2 Discos de freno 10” de 5 pernos|• 2 Mordazas|• 2 Soportes de mordaza|• Juego de rulimanes|&lt;br /&gt;|Estas cantidades sirven para un solo eje.</t>
   </si>
   <si>
     <t>Juego de Mangueras</t>
   </si>
   <si>
-    <t>Mangueras de freno termoplásticas con recubrimiento de peliuretano, anticorrosivas, para trabajos pesados ("heavy duty").|Incluye accesarios de conexión.|Medidas: 25' (7.62 m. Aprox.)/80" Ancho (2 m. Aprox.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accesarios </t>
+    <t>Mangueras de freno termoplásticas con recubrimiento de poliuretano, anticorrosivas, para trabajos pesados ("heavy duty").|Incluye accesarios de conexión.|Medidas: 25' (7.62 m. Aprox.)/80" Ancho (2 m. Aprox.)</t>
+  </si>
+  <si>
+    <t>Acoples</t>
   </si>
   <si>
     <t>accesorios</t>
   </si>
   <si>
-    <t>a. Acoples|b. Bolas|c. Alfombra sumergible|d. Engache y Tubo Recibidor.</t>
-  </si>
-  <si>
-    <t>Acoples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acople o Tortuga de 1 7/8"|Capacidad: 2000 - 3500 Lb.|Bola de 1 7/8"|Base 2" que se conecta al remolque.|Acople o Tortuga de 2" x 2"|Capacidad: 3500 Lb.|Bola de 2"|Base 2" que se conecta al remolque|Acople o Tortuga de 2" x 3"|Capacidad: 5000 Lb.|Bola 2"|Base 3" que se conecta al remolque </t>
+    <t>&lt;strong&gt;Diferentes medidas y capacidades:&lt;/strong&gt;|• 2000 Lb. Trabaja con bola 1 7/8”. Base que se conecta al remolque: 2”.|• 3500 Lb. Trabaja con bola 2”. Base que se conecta al remolque: 2”|• 5000 Lb. Trabaja con bola 2”. Base que se conecta al remolque: 3”</t>
   </si>
   <si>
     <t>Bolas de Acople</t>
   </si>
   <si>
-    <t>Bola de 1 7/8"|Capacidad: 2000 - 3500 Lb.|Bola de 2"|Capacidad: 3500 - 5000 Lb.|Bola de 2 5/16"|Capacidad: 1000 Lb.</t>
+    <t>&lt;strong&gt;Diferentes medidas y capacidades:&lt;/strong&gt;|• 1 7/8” – 2000 Lb.|• 2” - 3500 Lb.|• 2” - 5000 Lb.|• 2 5/16” – 40000 Lb.</t>
   </si>
   <si>
     <t>Alfombras Sumergibles</t>
   </si>
   <si>
-    <t>Para forrar las tablas de madera para deslizar las embarcaciones y facilitar su subida en el remolque.|No se deteriora con la salinidad del agua.|Se vende por metro.|Vienen en 2 medidas de ancho:|6 Pulgadas 30 cm. Aprox.|8 Pulgadas 45 cm. Aprox.</t>
+    <t>Para remolques de uso acuático. Se usa para forrar las tablas de madera por donde se deslizan las embarcaciones al subir al remolque.|No se deteriora con la salinidad.|Se venden por metro.|Diferentes medidas de ancho:|• 6” – 30 cm. aprox.|• 8” – 45 cm. aprox.</t>
   </si>
   <si>
     <t xml:space="preserve">Enganche y Tubo Recibidor </t>
   </si>
   <si>
-    <t>Enganche para Barra de Tubo|Para bola de 1 7/8, 2"|Capacidad: Hasta 2 toneladas se emperna al tubo recibidor.|Tubo Recibidor:|Cuadrado de 2"|Capacidad hasta 2 toneladas|Se suelda a la barra del tiro|Se venden por separado</t>
+    <t>Para la barra de tiro de su vehículo.|El Enganche trabaja con bolas 1 7/8” y 2”. Capacidad: 2 Ton. Se emperna al tubo recibidor.|El Tubo recibidor de 2”. Capacidad: 2 Ton. Se suelda en la barra de tiro.|Se venden por separado.</t>
   </si>
   <si>
     <t>Candado</t>
@@ -362,7 +341,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -377,6 +356,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1458,7 +1446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1468,8 +1456,8 @@
     <col min="2" max="2" width="42" style="1" customWidth="1"/>
     <col min="3" max="3" width="42.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="255" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.8516" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.25" customHeight="1">
@@ -1486,8 +1474,9 @@
         <v>2</v>
       </c>
       <c r="E1" s="2">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" ht="15.25" customHeight="1">
       <c r="A2" s="2">
@@ -1499,12 +1488,13 @@
       <c r="C2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" ht="15.25" customHeight="1">
       <c r="A3" s="2">
@@ -1516,12 +1506,13 @@
       <c r="C3" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s" s="3">
+      <c r="D3" t="s" s="5">
         <v>6</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" ht="15.25" customHeight="1">
       <c r="A4" s="2">
@@ -1533,12 +1524,13 @@
       <c r="C4" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D4" t="s" s="3">
+      <c r="D4" t="s" s="5">
         <v>8</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" ht="15.25" customHeight="1">
       <c r="A5" s="2">
@@ -1550,12 +1542,13 @@
       <c r="C5" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D5" t="s" s="3">
+      <c r="D5" t="s" s="5">
         <v>10</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" ht="15.25" customHeight="1">
       <c r="A6" s="2">
@@ -1565,709 +1558,609 @@
         <v>11</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s" s="3">
         <v>12</v>
       </c>
+      <c r="D6" t="s" s="5">
+        <v>13</v>
+      </c>
       <c r="E6" s="2">
         <v>0</v>
       </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" ht="15.25" customHeight="1">
       <c r="A7" s="2">
         <v>7</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>15</v>
+      </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" ht="15.25" customHeight="1">
       <c r="A8" s="2">
         <v>8</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s" s="3">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="D8" t="s" s="5">
+        <v>17</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
       </c>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" ht="15.25" customHeight="1">
       <c r="A9" s="2">
         <v>9</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s" s="3">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="D9" t="s" s="5">
+        <v>19</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" ht="15.25" customHeight="1">
       <c r="A10" s="2">
         <v>10</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>22</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" ht="15.25" customHeight="1">
       <c r="A11" s="2">
         <v>11</v>
       </c>
       <c r="B11" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="C11" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s" s="3">
-        <v>22</v>
+      <c r="D11" t="s" s="5">
+        <v>24</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" ht="15.25" customHeight="1">
       <c r="A12" s="2">
         <v>12</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" ht="15.25" customHeight="1">
       <c r="A13" s="2">
         <v>13</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s" s="3">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="D13" t="s" s="5">
+        <v>28</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
       </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" ht="15.25" customHeight="1">
       <c r="A14" s="2">
         <v>14</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s" s="3">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>30</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
       </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" ht="15.25" customHeight="1">
       <c r="A15" s="2">
         <v>15</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s" s="3">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="D15" t="s" s="5">
+        <v>32</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
       </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" ht="15.25" customHeight="1">
       <c r="A16" s="2">
         <v>16</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s" s="3">
-        <v>31</v>
+        <v>21</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>34</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
       </c>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" ht="15.25" customHeight="1">
       <c r="A17" s="2">
         <v>17</v>
       </c>
       <c r="B17" t="s" s="3">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s" s="3">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E17" s="2">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" ht="15.25" customHeight="1">
       <c r="A18" s="2">
         <v>18</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s" s="3">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="D18" t="s" s="5">
+        <v>39</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
       </c>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" ht="15.25" customHeight="1">
       <c r="A19" s="2">
         <v>19</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="D19" t="s" s="3">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="D19" t="s" s="5">
+        <v>41</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
       </c>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" ht="15.25" customHeight="1">
       <c r="A20" s="2">
         <v>20</v>
       </c>
       <c r="B20" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s" s="3">
         <v>36</v>
       </c>
-      <c r="C20" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="D20" t="s" s="3">
-        <v>37</v>
+      <c r="D20" t="s" s="5">
+        <v>43</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
       </c>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" ht="15.25" customHeight="1">
       <c r="A21" s="2">
         <v>21</v>
       </c>
       <c r="B21" t="s" s="3">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s" s="3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E21" s="2">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" ht="15.25" customHeight="1">
       <c r="A22" s="2">
         <v>22</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s" s="3">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
       </c>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" ht="15.25" customHeight="1">
       <c r="A23" s="2">
         <v>23</v>
       </c>
       <c r="B23" t="s" s="3">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s" s="3">
-        <v>39</v>
-      </c>
-      <c r="D23" t="s" s="3">
-        <v>43</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D23" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" ht="15.25" customHeight="1">
       <c r="A24" s="2">
         <v>24</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>39</v>
-      </c>
-      <c r="D24" t="s" s="3">
-        <v>45</v>
+        <v>36</v>
+      </c>
+      <c r="D24" t="s" s="5">
+        <v>51</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
       </c>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" ht="15.25" customHeight="1">
       <c r="A25" s="2">
         <v>25</v>
       </c>
       <c r="B25" t="s" s="3">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s" s="3">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s" s="3">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" ht="15.25" customHeight="1">
       <c r="A26" s="2">
         <v>26</v>
       </c>
       <c r="B26" t="s" s="3">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s" s="3">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" ht="15.25" customHeight="1">
       <c r="A27" s="2">
         <v>27</v>
       </c>
       <c r="B27" t="s" s="3">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s" s="3">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s" s="3">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
       </c>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" ht="15.25" customHeight="1">
       <c r="A28" s="2">
         <v>28</v>
       </c>
       <c r="B28" t="s" s="3">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>39</v>
-      </c>
-      <c r="D28" t="s" s="3">
-        <v>51</v>
+        <v>60</v>
+      </c>
+      <c r="D28" t="s" s="5">
+        <v>61</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" ht="15.25" customHeight="1">
       <c r="A29" s="2">
         <v>29</v>
       </c>
       <c r="B29" t="s" s="3">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>39</v>
-      </c>
-      <c r="D29" t="s" s="3">
-        <v>52</v>
+        <v>60</v>
+      </c>
+      <c r="D29" t="s" s="5">
+        <v>63</v>
       </c>
       <c r="E29" s="2">
         <v>0</v>
       </c>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" ht="15.25" customHeight="1">
       <c r="A30" s="2">
         <v>30</v>
       </c>
-      <c r="B30" t="s" s="3">
-        <v>53</v>
+      <c r="B30" t="s" s="5">
+        <v>64</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>54</v>
-      </c>
-      <c r="D30" t="s" s="3">
-        <v>55</v>
+        <v>65</v>
+      </c>
+      <c r="D30" t="s" s="5">
+        <v>66</v>
       </c>
       <c r="E30" s="2">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" ht="15.25" customHeight="1">
       <c r="A31" s="2">
         <v>31</v>
       </c>
       <c r="B31" t="s" s="3">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s" s="3">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s" s="3">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
       </c>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" ht="15.25" customHeight="1">
       <c r="A32" s="2">
         <v>32</v>
       </c>
       <c r="B32" t="s" s="3">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s" s="3">
-        <v>54</v>
-      </c>
-      <c r="D32" t="s" s="3">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="D32" t="s" s="5">
+        <v>70</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
       </c>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" ht="15.25" customHeight="1">
       <c r="A33" s="2">
         <v>33</v>
       </c>
       <c r="B33" t="s" s="3">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s" s="3">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D33" t="s" s="3">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E33" s="2">
         <v>0</v>
       </c>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" ht="15.25" customHeight="1">
       <c r="A34" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s" s="3">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s" s="3">
-        <v>63</v>
-      </c>
-      <c r="D34" t="s" s="3">
-        <v>64</v>
+        <v>74</v>
+      </c>
+      <c r="D34" t="s" s="5">
+        <v>75</v>
       </c>
       <c r="E34" s="2">
         <v>1</v>
       </c>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" ht="15.25" customHeight="1">
       <c r="A35" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s" s="3">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s" s="3">
-        <v>63</v>
-      </c>
-      <c r="D35" t="s" s="3">
-        <v>66</v>
+        <v>74</v>
+      </c>
+      <c r="D35" t="s" s="5">
+        <v>77</v>
       </c>
       <c r="E35" s="2">
         <v>0</v>
       </c>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" ht="15.25" customHeight="1">
       <c r="A36" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s" s="3">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s" s="3">
-        <v>63</v>
-      </c>
-      <c r="D36" t="s" s="3">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="D36" t="s" s="5">
+        <v>79</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
       </c>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" ht="15.25" customHeight="1">
       <c r="A37" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s" s="3">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C37" t="s" s="3">
-        <v>70</v>
-      </c>
-      <c r="D37" t="s" s="3">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="D37" t="s" s="5">
+        <v>81</v>
       </c>
       <c r="E37" s="2">
         <v>0</v>
       </c>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" ht="15.25" customHeight="1">
       <c r="A38" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s" s="3">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s" s="3">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D38" t="s" s="3">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E38" s="2">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" ht="15.25" customHeight="1">
       <c r="A39" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s" s="3">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s" s="3">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D39" t="s" s="3">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="E39" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" ht="15.25" customHeight="1">
-      <c r="A40" s="2">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s" s="3">
-        <v>76</v>
-      </c>
-      <c r="C40" t="s" s="3">
-        <v>70</v>
-      </c>
-      <c r="D40" t="s" s="3">
-        <v>77</v>
-      </c>
-      <c r="E40" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" ht="15.25" customHeight="1">
-      <c r="A41" s="2">
-        <v>41</v>
-      </c>
-      <c r="B41" t="s" s="3">
-        <v>78</v>
-      </c>
-      <c r="C41" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="D41" t="s" s="3">
-        <v>80</v>
-      </c>
-      <c r="E41" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" ht="15.25" customHeight="1">
-      <c r="A42" s="2">
-        <v>42</v>
-      </c>
-      <c r="B42" t="s" s="3">
-        <v>81</v>
-      </c>
-      <c r="C42" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="D42" t="s" s="3">
-        <v>82</v>
-      </c>
-      <c r="E42" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" ht="15.25" customHeight="1">
-      <c r="A43" s="2">
-        <v>43</v>
-      </c>
-      <c r="B43" t="s" s="3">
-        <v>83</v>
-      </c>
-      <c r="C43" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="D43" t="s" s="3">
-        <v>84</v>
-      </c>
-      <c r="E43" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" ht="15.25" customHeight="1">
-      <c r="A44" s="2">
-        <v>44</v>
-      </c>
-      <c r="B44" t="s" s="3">
-        <v>85</v>
-      </c>
-      <c r="C44" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="D44" t="s" s="3">
-        <v>86</v>
-      </c>
-      <c r="E44" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" ht="15.25" customHeight="1">
-      <c r="A45" s="2">
-        <v>45</v>
-      </c>
-      <c r="B45" t="s" s="3">
-        <v>87</v>
-      </c>
-      <c r="C45" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="D45" t="s" s="3">
-        <v>88</v>
-      </c>
-      <c r="E45" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" ht="15.25" customHeight="1">
-      <c r="A46" s="2">
-        <v>46</v>
-      </c>
-      <c r="B46" t="s" s="3">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="D46" t="s" s="3">
-        <v>90</v>
-      </c>
-      <c r="E46" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" ht="15.25" customHeight="1">
-      <c r="A47" s="2">
-        <v>47</v>
-      </c>
-      <c r="B47" t="s" s="3">
-        <v>91</v>
-      </c>
-      <c r="C47" t="s" s="3">
-        <v>92</v>
-      </c>
-      <c r="D47" t="s" s="3">
-        <v>93</v>
-      </c>
-      <c r="E47" s="2">
-        <v>1</v>
-      </c>
+      <c r="F39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizamos la lista de productos
</commit_message>
<xml_diff>
--- a/assets/php/listado.xlsx
+++ b/assets/php/listado.xlsx
@@ -11,14 +11,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="97">
+  <si>
+    <t>Características</t>
+  </si>
+  <si>
+    <t>torsion</t>
+  </si>
+  <si>
+    <t>Suspensión hexagonal de caucho con suspensión independiente que asegura una transportación cuidadosa y segura.|&lt;br /&gt;|Durante la suspensión no se aplastan las gomas, sino que tienen espacio para trabajar (flexión), lo que asegura una amortiguación propia, suave y más estable, en cada rueda, logrando que las irregularidades de la carretera solo afecten el lado en que se originan.</t>
+  </si>
   <si>
     <t>Eje de Torsión 4 Pernos 750 Kg.</t>
   </si>
   <si>
-    <t>torsion</t>
-  </si>
-  <si>
     <t>Marca: AL-KO|Capacidad: 750 Kg. (1650 Lb.)|Fácil Instalación|Se adhiere al chasis mediante 8 pernos.|Garantía: 2 años.|&lt;br /&gt;|Al usar este eje de torsión, &lt;strong&gt;NO NECESITA&lt;/strong&gt;|• Paquetes de resorte|• Platineras|• Abrazaderas|• Orejas|• Uniones|• Monturitas|&lt;br /&gt;|&lt;strong&gt;BENEFICIOS:&lt;/strong&gt;|✓Amortiguación suave|✓Mayor estabilidad a mayor velocidad|✓No salta la carga|✓Se elimina el tiempo de armado y suelda del eje en el sistema convencional</t>
   </si>
   <si>
@@ -46,12 +52,15 @@
     <t xml:space="preserve">Tramo de tubo exterior hexagonal para alargar ejes de torsión de 750 Kg.|Galvanizado en caliente.|Marca: AL-KO </t>
   </si>
   <si>
+    <t>punta</t>
+  </si>
+  <si>
+    <t>Determina la capacidad de carga de su remolque. Es importante considerar no solo el peso de su carga sino también el peso de su remolque al momento de elegirlo.|&lt;br /&gt;|&lt;strong&gt;Comprende:&lt;/strong&gt;|• Manzana|• Rulimanes|• Retenedor|• Tapa grasera|• Tuercas de seguridad aceradas|• Seguro|• Punta con tuerca y arandela|&lt;br /&gt;|Se necesitan 2 Kits de punta de eje para armar un eje.</t>
+  </si>
+  <si>
     <t>Kit de Punta de Eje 4 Pernos 1000 Lb.</t>
   </si>
   <si>
-    <t>punta</t>
-  </si>
-  <si>
     <t>Distancia entre pernos: 4" (10 cm. Aprox.)|Se necesitan 2 Kits para armar un eje de 2000 Lb.|Trabaja con aros de 12”, 13”, 14".</t>
   </si>
   <si>
@@ -73,12 +82,15 @@
     <t xml:space="preserve">Distancia entre pernos: 5.5" (14 cm. Aprox.)|Se necesitan 2 Kits para armar un eje de 6000 Lb.|Trabaja con aros de 14”, 15”, 16". </t>
   </si>
   <si>
+    <t>suspension</t>
+  </si>
+  <si>
+    <t>Sistemas de suspensión clásica utilizada en remolques.|Los Paquetes de resorte (muelles) sirven como amortiguador en el remolque.|Pueden ser de un solo ojo (deslizantes), o de doble ojo.|Su capacidad debe ir acorde a la capacidad de los kits de punta de eje de su remolque.</t>
+  </si>
+  <si>
     <t>Paquetes de Resorte 1650 Lb.</t>
   </si>
   <si>
-    <t>suspension</t>
-  </si>
-  <si>
     <t>Capacidad: 1650 Lb.|Largo: 24” (60.96 cm.)|Ancho: 1 3⁄4” (4.45 cm.)|(La distancia se mide del centro del ojo hasta el centro del final de la hoja.)</t>
   </si>
   <si>
@@ -118,12 +130,15 @@
     <t>Sistema para instalar paquetes de resorte en remolques de doble eje.|&lt;br /&gt;|&lt;strong&gt;Comprende:&lt;/strong&gt;|• 4 Orejas delanteras 1 3⁄4” X 1 1⁄2”|• 2 Orejas de balance 2 1⁄4”|• 2 Triángulos de balance 7 3⁄4”|• 8 Platineras 1 1⁄2” x 1⁄4”|• 14 Pernos 1/2” x 3 1/2”|• 14 Tuercas 1/2|Se necesita 1 solo kit para instalar 4 paquetes.|No incluye paquetes de Resorte.</t>
   </si>
   <si>
+    <t>patas</t>
+  </si>
+  <si>
+    <t>Sencillo pero necesario componente que consiste en un tubo rígido con una manivela que permite ajustar la altura del remolque.|Pueden ser con rueda, o estacionarias.|Cuando hay que desplazar el remolque se recomienda elevar la rueda todo lo posible.</t>
+  </si>
+  <si>
     <t>Patas de Soporte con Rueda - 1000 Lb.</t>
   </si>
   <si>
-    <t>patas</t>
-  </si>
-  <si>
     <t>Con rueda plástica.|&lt;strong&gt;Medidas:&lt;strong&gt;|23” (58.42 cm.) en estado normal|34” (86.36 cm.) extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|• Facilita el enganche en el sistema del carro, ya que permite subir y bajar el remolque en un margen de 40 cm.|• Sirve como apoyo cuando el remolque está estacionado.|• Permite arrastrar el remolque con menor esfuerzo, ya que se sostiene sobre la rueda.</t>
   </si>
   <si>
@@ -169,12 +184,15 @@
     <t>Con base cuadrada. Galvanizada.|Viene con pernos y platinas para instalar en el remolque.|&lt;strong&gt;Medidas:&lt;strong&gt;|24.5” (62.23 cm.) en estado normal|40” (101.60 cm.) extendida.|&lt;br /&gt;|&lt;strong&gt;Utilidades:&lt;strong&gt;|• Sube y baja 40 cm. Aprox.|• Sirve como apoyo cuando el remolque está estacionado.</t>
   </si>
   <si>
+    <t>aros</t>
+  </si>
+  <si>
+    <t>De diferentes medidas y capacidades para uso en remolques.</t>
+  </si>
+  <si>
     <t>Aros con Llanta 8</t>
   </si>
   <si>
-    <t>aros</t>
-  </si>
-  <si>
     <t>4 Huecos|Medida llanta: 4.80 x 8.|Capacidad 585 Lb.|Aro Blanco</t>
   </si>
   <si>
@@ -190,12 +208,15 @@
     <t>5 Huecos|Medida llanta: ST205/75D14|Capacidad 1760 Lb.|Aro Blanco</t>
   </si>
   <si>
+    <t>guardafangos</t>
+  </si>
+  <si>
+    <t>Marca AL-KO|Plásticos, resistentes y elegantes.|Para remolques de un eje, y de doble eje.</t>
+  </si>
+  <si>
     <t>Guardafangos Sencillos</t>
   </si>
   <si>
-    <t>guardafangos</t>
-  </si>
-  <si>
     <t>Para un solo eje.|Marca: AL-KO.|Material: plástico|Trabajan con aro 13” y 14”. Largo 73 cm.|Ancho 20 cm.|Profundidad 36 cm.</t>
   </si>
   <si>
@@ -205,12 +226,15 @@
     <t>Para doble eje.|Marca: AL-KO.|Material: plástico|Trabajan con aro 13” y 14”. Largo 146 cm.|Ancho 22 cm. Profundidad 36 cm.</t>
   </si>
   <si>
+    <t>frenos</t>
+  </si>
+  <si>
+    <t>El Sistema de freno hidráulico inercial en un remolque es conveniente por su simplicidad, confiabilidad, facilidad de mantenimiento y alta eficacia.|&lt;br /&gt;|&lt;strong&gt;Un Sistema de freno clásico comprende:&lt;/strong&gt;|• Acople de freno|• Kit de Frenos de disco|• Puntas de eje con bridas|• Mangueras</t>
+  </si>
+  <si>
     <t>Acople de freno</t>
   </si>
   <si>
-    <t>frenos</t>
-  </si>
-  <si>
     <t>Capacidad 7000 Lb. (3.1 Ton.)|Trabaja con bola 2”.|Solenoide incorporado al cilindro maestro, que facilita la revisión sin sacar la línea de frenado.|Con pin de seguridad para la bola, y cable de freno recubierto en PVC.</t>
   </si>
   <si>
@@ -232,12 +256,15 @@
     <t>Mangueras de freno termoplásticas con recubrimiento de poliuretano, anticorrosivas, para trabajos pesados ("heavy duty").|Incluye accesarios de conexión.|Medidas: 25' (7.62 m. Aprox.)/80" Ancho (2 m. Aprox.)</t>
   </si>
   <si>
+    <t>accesorios</t>
+  </si>
+  <si>
+    <t>• Acoples|• Bolas|• Tubo recibidor y enganche|• Alfombras|• Candados</t>
+  </si>
+  <si>
     <t>Acoples</t>
   </si>
   <si>
-    <t>accesorios</t>
-  </si>
-  <si>
     <t>&lt;strong&gt;Diferentes medidas y capacidades:&lt;/strong&gt;|• 2000 Lb. Trabaja con bola 1 7/8”. Base que se conecta al remolque: 2”.|• 3500 Lb. Trabaja con bola 2”. Base que se conecta al remolque: 2”|• 5000 Lb. Trabaja con bola 2”. Base que se conecta al remolque: 3”</t>
   </si>
   <si>
@@ -265,10 +292,13 @@
     <t>Candado para tubo recibidor</t>
   </si>
   <si>
+    <t>chasis</t>
+  </si>
+  <si>
+    <t>Los mejores Chasis, nuevos modelos próximamente</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chasis </t>
-  </si>
-  <si>
-    <t>chasis</t>
   </si>
   <si>
     <t>a. Chasis</t>
@@ -354,11 +384,11 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
@@ -1446,7 +1476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1470,13 +1500,11 @@
       <c r="C1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
-        <v>0</v>
-      </c>
-      <c r="F1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" ht="15.25" customHeight="1">
       <c r="A2" s="2">
@@ -1488,13 +1516,13 @@
       <c r="C2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" t="s" s="3">
         <v>4</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" ht="15.25" customHeight="1">
       <c r="A3" s="2">
@@ -1506,13 +1534,13 @@
       <c r="C3" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="D3" t="s" s="4">
         <v>6</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" ht="15.25" customHeight="1">
       <c r="A4" s="2">
@@ -1524,13 +1552,13 @@
       <c r="C4" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D4" t="s" s="5">
+      <c r="D4" t="s" s="4">
         <v>8</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" ht="15.25" customHeight="1">
       <c r="A5" s="2">
@@ -1542,13 +1570,13 @@
       <c r="C5" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D5" t="s" s="5">
+      <c r="D5" t="s" s="4">
         <v>10</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" ht="15.25" customHeight="1">
       <c r="A6" s="2">
@@ -1558,609 +1586,755 @@
         <v>11</v>
       </c>
       <c r="C6" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="D6" t="s" s="5">
-        <v>13</v>
-      </c>
       <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" ht="15.25" customHeight="1">
       <c r="A7" s="2">
         <v>7</v>
       </c>
       <c r="B7" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="C7" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" ht="15.25" customHeight="1">
       <c r="A8" s="2">
         <v>8</v>
       </c>
       <c r="B8" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="C8" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s" s="5">
-        <v>17</v>
-      </c>
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" ht="15.25" customHeight="1">
       <c r="A9" s="2">
         <v>9</v>
       </c>
       <c r="B9" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="C9" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s" s="5">
-        <v>19</v>
-      </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" ht="15.25" customHeight="1">
       <c r="A10" s="2">
         <v>10</v>
       </c>
       <c r="B10" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="C10" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s" s="5">
-        <v>22</v>
-      </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" ht="15.25" customHeight="1">
       <c r="A11" s="2">
         <v>11</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s" s="5">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="D11" t="s" s="4">
+        <v>22</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" ht="15.25" customHeight="1">
       <c r="A12" s="2">
         <v>12</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D12" t="s" s="4">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" ht="15.25" customHeight="1">
       <c r="A13" s="2">
         <v>13</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s" s="5">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="D13" t="s" s="4">
+        <v>26</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" ht="15.25" customHeight="1">
       <c r="A14" s="2">
         <v>14</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s" s="5">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="D14" t="s" s="4">
+        <v>28</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" ht="15.25" customHeight="1">
       <c r="A15" s="2">
         <v>15</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s" s="5">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="D15" t="s" s="3">
+        <v>30</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" ht="15.25" customHeight="1">
       <c r="A16" s="2">
         <v>16</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D16" t="s" s="5">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="D16" t="s" s="4">
+        <v>32</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" ht="15.25" customHeight="1">
       <c r="A17" s="2">
         <v>17</v>
       </c>
       <c r="B17" t="s" s="3">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s" s="3">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="D17" t="s" s="4">
+        <v>34</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" ht="15.25" customHeight="1">
       <c r="A18" s="2">
         <v>18</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s" s="4">
         <v>36</v>
       </c>
-      <c r="D18" t="s" s="5">
-        <v>39</v>
-      </c>
       <c r="E18" s="2">
         <v>0</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" ht="15.25" customHeight="1">
       <c r="A19" s="2">
         <v>19</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s" s="5">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="D19" t="s" s="4">
+        <v>38</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" ht="15.25" customHeight="1">
       <c r="A20" s="2">
         <v>20</v>
       </c>
       <c r="B20" t="s" s="3">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="C20" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D20" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" ht="15.25" customHeight="1">
       <c r="A21" s="2">
         <v>21</v>
       </c>
       <c r="B21" t="s" s="3">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s" s="3">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" ht="15.25" customHeight="1">
       <c r="A22" s="2">
         <v>22</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="D22" t="s" s="3">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="D22" t="s" s="4">
+        <v>44</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" ht="15.25" customHeight="1">
       <c r="A23" s="2">
         <v>23</v>
       </c>
       <c r="B23" t="s" s="3">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s" s="5">
-        <v>49</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1</v>
-      </c>
-      <c r="F23" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D23" t="s" s="4">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" ht="15.25" customHeight="1">
       <c r="A24" s="2">
         <v>24</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="D24" t="s" s="5">
-        <v>51</v>
+        <v>39</v>
+      </c>
+      <c r="D24" t="s" s="4">
+        <v>48</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
       </c>
-      <c r="F24" s="4"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" ht="15.25" customHeight="1">
       <c r="A25" s="2">
         <v>25</v>
       </c>
       <c r="B25" t="s" s="3">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s" s="3">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s" s="3">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" ht="15.25" customHeight="1">
       <c r="A26" s="2">
         <v>26</v>
       </c>
       <c r="B26" t="s" s="3">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s" s="3">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
-      <c r="F26" s="4"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" ht="15.25" customHeight="1">
       <c r="A27" s="2">
         <v>27</v>
       </c>
       <c r="B27" t="s" s="3">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s" s="3">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s" s="3">
-        <v>58</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D27" t="s" s="4">
+        <v>54</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" ht="15.25" customHeight="1">
       <c r="A28" s="2">
         <v>28</v>
       </c>
       <c r="B28" t="s" s="3">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>60</v>
-      </c>
-      <c r="D28" t="s" s="5">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="D28" t="s" s="4">
+        <v>56</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" ht="15.25" customHeight="1">
       <c r="A29" s="2">
         <v>29</v>
       </c>
       <c r="B29" t="s" s="3">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>60</v>
-      </c>
-      <c r="D29" t="s" s="5">
-        <v>63</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="D29" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" ht="15.25" customHeight="1">
       <c r="A30" s="2">
         <v>30</v>
       </c>
-      <c r="B30" t="s" s="5">
-        <v>64</v>
+      <c r="B30" t="s" s="3">
+        <v>59</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>65</v>
-      </c>
-      <c r="D30" t="s" s="5">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="D30" t="s" s="3">
+        <v>60</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" ht="15.25" customHeight="1">
       <c r="A31" s="2">
         <v>31</v>
       </c>
       <c r="B31" t="s" s="3">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s" s="3">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s" s="3">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" ht="15.25" customHeight="1">
       <c r="A32" s="2">
         <v>32</v>
       </c>
       <c r="B32" t="s" s="3">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s" s="3">
-        <v>65</v>
-      </c>
-      <c r="D32" t="s" s="5">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="D32" t="s" s="3">
+        <v>64</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" ht="15.25" customHeight="1">
       <c r="A33" s="2">
         <v>33</v>
       </c>
       <c r="B33" t="s" s="3">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s" s="3">
         <v>65</v>
       </c>
-      <c r="D33" t="s" s="3">
-        <v>72</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4"/>
+      <c r="D33" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" ht="15.25" customHeight="1">
       <c r="A34" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s" s="3">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s" s="3">
-        <v>74</v>
-      </c>
-      <c r="D34" t="s" s="5">
-        <v>75</v>
+        <v>65</v>
+      </c>
+      <c r="D34" t="s" s="4">
+        <v>68</v>
       </c>
       <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="F34" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" ht="15.25" customHeight="1">
       <c r="A35" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s" s="3">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s" s="3">
-        <v>74</v>
-      </c>
-      <c r="D35" t="s" s="5">
-        <v>77</v>
+        <v>65</v>
+      </c>
+      <c r="D35" t="s" s="4">
+        <v>70</v>
       </c>
       <c r="E35" s="2">
         <v>0</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" ht="15.25" customHeight="1">
       <c r="A36" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s" s="3">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="C36" t="s" s="3">
-        <v>74</v>
-      </c>
-      <c r="D36" t="s" s="5">
-        <v>79</v>
-      </c>
-      <c r="E36" s="2">
-        <v>0</v>
-      </c>
-      <c r="F36" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="D36" t="s" s="4">
+        <v>72</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" ht="15.25" customHeight="1">
       <c r="A37" s="2">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s" s="3">
-        <v>80</v>
+        <v>37</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>73</v>
       </c>
       <c r="C37" t="s" s="3">
+        <v>71</v>
+      </c>
+      <c r="D37" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="D37" t="s" s="5">
-        <v>81</v>
-      </c>
       <c r="E37" s="2">
         <v>0</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" ht="15.25" customHeight="1">
       <c r="A38" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s" s="3">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s" s="3">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s" s="3">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" ht="15.25" customHeight="1">
       <c r="A39" s="2">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s" s="3">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s" s="3">
+        <v>71</v>
+      </c>
+      <c r="D39" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" ht="15.25" customHeight="1">
+      <c r="A40" s="2">
         <v>40</v>
       </c>
-      <c r="B39" t="s" s="3">
+      <c r="B40" t="s" s="3">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s" s="3">
+        <v>71</v>
+      </c>
+      <c r="D40" t="s" s="3">
+        <v>80</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" ht="15.25" customHeight="1">
+      <c r="A41" s="2">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="D41" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" ht="15.25" customHeight="1">
+      <c r="A42" s="2">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="D42" t="s" s="4">
         <v>84</v>
       </c>
-      <c r="C39" t="s" s="3">
+      <c r="E42" s="2">
+        <v>1</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" ht="15.25" customHeight="1">
+      <c r="A43" s="2">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s" s="3">
         <v>85</v>
       </c>
-      <c r="D39" t="s" s="3">
+      <c r="C43" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s" s="4">
         <v>86</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" ht="15.25" customHeight="1">
+      <c r="A44" s="2">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s" s="3">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s" s="4">
+        <v>88</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" ht="15.25" customHeight="1">
+      <c r="A45" s="2">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s" s="3">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="D45" t="s" s="4">
+        <v>90</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" ht="15.25" customHeight="1">
+      <c r="A46" s="2">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s" s="3">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="D46" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="E46" s="2">
         <v>1</v>
       </c>
-      <c r="F39" s="4"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" ht="15.25" customHeight="1">
+      <c r="A47" s="2">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s" s="3">
+        <v>93</v>
+      </c>
+      <c r="D47" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" ht="15.25" customHeight="1">
+      <c r="A48" s="2">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s" s="3">
+        <v>95</v>
+      </c>
+      <c r="C48" t="s" s="3">
+        <v>93</v>
+      </c>
+      <c r="D48" t="s" s="3">
+        <v>96</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>